<commit_message>
feat: Added lone ranger method for rows and columns, optimizing by a factor of 10 process time of solution. docs updated with the new results in page V3.
</commit_message>
<xml_diff>
--- a/docs/Sudoku results by version.xlsx
+++ b/docs/Sudoku results by version.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebad\Desktop\HPC-SudokuThreads\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F226F6C-719F-4153-B50E-03B47230B0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07798771-455C-4726-BB75-B1F544E3F7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" activeTab="1" xr2:uid="{615442DA-7042-448C-BD41-E92EAD2F62D2}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" activeTab="2" xr2:uid="{615442DA-7042-448C-BD41-E92EAD2F62D2}"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="1" r:id="rId1"/>
     <sheet name="V2" sheetId="2" r:id="rId2"/>
+    <sheet name="V3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>Cores</t>
   </si>
@@ -53,6 +54,9 @@
   </si>
   <si>
     <t>ANALISIS SUDOKU 16x16 HARD (V2)</t>
+  </si>
+  <si>
+    <t>ANALISIS SUDOKU 16x16 HARD (V3)</t>
   </si>
 </sst>
 </file>
@@ -2898,6 +2902,1397 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CL" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Grafico speedUp vs Eficiencia</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-CL">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'V3'!$E$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speedup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'V3'!$C$8:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'V3'!$E$8:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94692434866883302</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89056887030186049</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0336029869321717</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2393672586181168</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6754085132136374</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8315139486161649</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.257713742014408</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4958677685950414</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4009829430471235</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2904026475455046</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1749378028021473</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.0945775535939468</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D749-44CC-96C6-14EEBD076514}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'V3'!$F$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Eficiencia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'V3'!$C$8:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'V3'!$F$8:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.47346217433441651</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29685629010062015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25840074673304292</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24787345172362335</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2792347522022729</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26164484980230929</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.282214217751801</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.27731864095500458</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24009829430471236</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.20821842250413677</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.18124481690017893</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.16112135027645744</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D749-44CC-96C6-14EEBD076514}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1315398976"/>
+        <c:axId val="1315399808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1315398976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1315399808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1315399808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1315398976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CL"/>
+              <a:t>Eficiencia vs</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-CL" baseline="0"/>
+              <a:t> Cores</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'V3'!$F$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Eficiencia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'V3'!$C$8:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'V3'!$F$8:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.47346217433441651</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29685629010062015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25840074673304292</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24787345172362335</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2792347522022729</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26164484980230929</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.282214217751801</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.27731864095500458</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24009829430471236</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.20821842250413677</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.18124481690017893</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.16112135027645744</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8894-4760-BF61-C2FB5FBAA927}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1415517280"/>
+        <c:axId val="1415513536"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1415517280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1415513536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1415513536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1415517280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CL"/>
+              <a:t>Speedup vs Cores</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'V3'!$E$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speedup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'V3'!$C$8:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'V3'!$E$8:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94692434866883302</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89056887030186049</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0336029869321717</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2393672586181168</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6754085132136374</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8315139486161649</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.257713742014408</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4958677685950414</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4009829430471235</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2904026475455046</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1749378028021473</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.0945775535939468</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E006-45F2-B7C8-85156C5202E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1375880800"/>
+        <c:axId val="1375878304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1375880800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1375878304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1375878304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1375880800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3138,6 +4533,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5719,6 +7234,1554 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6460,6 +9523,119 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66501</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>178723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>315883</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>54032</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Gráfico 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32351899-BDE9-4CDA-A7C3-72F3F100BEDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>162097</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>411479</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>12469</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Gráfico 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E93BE5B1-C30A-4782-88DA-BF098DBDFB4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>669174</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>37407</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>54032</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>103909</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Gráfico 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90E13E6E-BF58-4A78-BFDA-66055F76FD4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -7029,8 +10205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC4573E-4463-49A6-903C-E03DFC1C7629}">
   <dimension ref="C5:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -7278,7 +10454,275 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370D7BB8-335F-43AA-91EF-AFE79B802830}">
+  <dimension ref="C5:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>16610</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>17541</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" ref="E9:E20" si="0">$D$8/D9</f>
+        <v>0.94692434866883302</v>
+      </c>
+      <c r="F9" s="5">
+        <f>E9/C9</f>
+        <v>0.47346217433441651</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="2">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2">
+        <v>18651</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.89056887030186049</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" ref="F10:F20" si="1">E10/C10</f>
+        <v>0.29685629010062015</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>16070</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0336029869321717</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" si="1"/>
+        <v>0.25840074673304292</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>13402</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2393672586181168</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="1"/>
+        <v>0.24787345172362335</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="2">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2">
+        <v>9914</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6754085132136374</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="1"/>
+        <v>0.2792347522022729</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="2">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2">
+        <v>9069</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
+        <v>1.8315139486161649</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="1"/>
+        <v>0.26164484980230929</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="2">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2">
+        <v>7357</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="0"/>
+        <v>2.257713742014408</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="1"/>
+        <v>0.282214217751801</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="2">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2">
+        <v>6655</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="0"/>
+        <v>2.4958677685950414</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="1"/>
+        <v>0.27731864095500458</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="2">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2">
+        <v>6918</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
+        <v>2.4009829430471235</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="1"/>
+        <v>0.24009829430471236</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="2">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2">
+        <v>7252</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="0"/>
+        <v>2.2904026475455046</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="1"/>
+        <v>0.20821842250413677</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="2">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2">
+        <v>7637</v>
+      </c>
+      <c r="E19" s="7">
+        <f>$D$8/D19</f>
+        <v>2.1749378028021473</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" si="1"/>
+        <v>0.18124481690017893</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="2">
+        <v>13</v>
+      </c>
+      <c r="D20" s="2">
+        <v>7930</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="0"/>
+        <v>2.0945775535939468</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" si="1"/>
+        <v>0.16112135027645744</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C5:F6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010074BFCFE3E55FA246A33CA5520A73FC55" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="982f60e662a9819f36334c485bc0ef2c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b1034983-80d7-443b-afbb-f8559efcc122" xmlns:ns4="17f3baef-38ff-4830-8ea2-808664c07c07" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="292736758e5298b5b23fd7e7aca38269" ns3:_="" ns4:_="">
     <xsd:import namespace="b1034983-80d7-443b-afbb-f8559efcc122"/>
@@ -7489,22 +10933,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD134A20-B6B1-43C9-9969-5E9523C51E8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="17f3baef-38ff-4830-8ea2-808664c07c07"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b1034983-80d7-443b-afbb-f8559efcc122"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D235676A-7AB1-43AC-84EF-EC6036E00148}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACA06D96-14B0-4D53-874D-74CC0BE45A96}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7521,29 +10975,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D235676A-7AB1-43AC-84EF-EC6036E00148}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD134A20-B6B1-43C9-9969-5E9523C51E8D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="17f3baef-38ff-4830-8ea2-808664c07c07"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b1034983-80d7-443b-afbb-f8559efcc122"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>